<commit_message>
Changes made to Summary file and certain code
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\code\The 75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E20C695-B6E7-4EC7-B942-0E4D933E9512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2058AD-3DC4-451C-B999-E1D9C8350E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,11 +43,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Create a HashMap. For each element search for it's compliement in map as a key. If it doesn't contain store the current number and it's index(k:v). If found return index of current number and return value 
-from map (map.get(compliment))
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">For a given integer array, return true if it contains a duplicate. Otherwise return false </t>
   </si>
   <si>
@@ -79,10 +74,6 @@
 the end of the output and the stack is empty, return true.</t>
   </si>
   <si>
-    <t xml:space="preserve">Given an array, return the maximum sum a possible subarray can have. 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kadane's algorithm. Compare two things, the sum of the current subarray and the current element. If the current
 element is larger then the sum of the current subarray+current element, create a new subarray with just the current 
 element. Keep track of running max after each iteration. </t>
@@ -90,11 +81,6 @@
   <si>
     <t>Given an integer array, return an array where for each element shows the producte of the array
 except for itself. *Can't use division*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Idea is the answer is products to the left X products to the right.  Calculate the products toTheLeftOf and place into
-output array. With the first element being one. Can use an array to represent toTheRightOf or variable with starting
-value 1.  For each element multiply toTheLeftOf with toTheRightOf to get the result. </t>
   </si>
   <si>
     <t>TwoSum 1</t>
@@ -141,18 +127,30 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Sort the array based on the low values. Create and output arrayList and add the first interval onto it. Iterate through
-the input array and compare the current high value with the next low. If the current high value is larger then the next
-low, merge the two intervals by taking the max of both intertval high values.  If no overlapping update add intervall to
-output array and update current interval. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Given an array of Strings, return a list of arrays with where a given array is anagrams of eachother </t>
   </si>
   <si>
     <t xml:space="preserve">Sort the words. All anagrams will be equal once sorted. Map the sorted words to all it's anagrams with the sorted word
 being the key. If the sorted word isn't in map, add sorted as key and the corresponding string as an anagram.  Use addAll
 Operation to add map.values() to output array. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a HashMap. For each element search for it's compliement in map as a key. If map doesn't contain compliment store the current element and it's index into map(k:v). If found in map, return index of current number and return value from map (map.get(compliment))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given an array, return the maximum sum a possible subarray can have. 
+Ex. Input = {-2, 1, -3, 4, -1, 2, 1, -5, 4}  output = 6 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The answer for a given element is products to the left of it  multiplied by products to the right it.  Calculate the products toTheLeftOf and place into output array. With the first element being one. Can use an array to represent toTheRightOf or variable with starting value 1.  For each element multiply toTheLeftOf with toTheRightOf to get the result. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort the array based on the low values. Create an output arrayList and add the first interval onto it. Iterate through
+the input array and compare the current high value with the next low. If the current high value is larger then the next
+low, merge the two intervals by taking the max of both intertval high values.  If no overlapping add interval to
+output array and update current interval. </t>
   </si>
 </sst>
 </file>
@@ -195,16 +193,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,143 +516,143 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Wrapped up week1 changes
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\code\The 75\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2058AD-3DC4-451C-B999-E1D9C8350E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7826A96-9FD1-4B11-ACB7-3787B0B59038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,13 +123,6 @@
 to change low value and the algorithm will change the high to compute the correct sum. </t>
   </si>
   <si>
-    <t xml:space="preserve">Given an array of Intervals, merge any overlapping intervals and return the output array. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given an array of Strings, return a list of arrays with where a given array is anagrams of eachother </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sort the words. All anagrams will be equal once sorted. Map the sorted words to all it's anagrams with the sorted word
 being the key. If the sorted word isn't in map, add sorted as key and the corresponding string as an anagram.  Use addAll
 Operation to add map.values() to output array. </t>
@@ -147,10 +140,17 @@
     <t xml:space="preserve">The answer for a given element is products to the left of it  multiplied by products to the right it.  Calculate the products toTheLeftOf and place into output array. With the first element being one. Can use an array to represent toTheRightOf or variable with starting value 1.  For each element multiply toTheLeftOf with toTheRightOf to get the result. </t>
   </si>
   <si>
-    <t xml:space="preserve">Sort the array based on the low values. Create an output arrayList and add the first interval onto it. Iterate through
-the input array and compare the current high value with the next low. If the current high value is larger then the next
-low, merge the two intervals by taking the max of both intertval high values.  If no overlapping add interval to
-output array and update current interval. </t>
+    <t>Given an array of Intervals, merge any overlapping intervals and return the output array. 
+Ex. Input = {{1,3}, {2, 6}, {8, 10}, {15, 18}} Output = {{1, 6}, {8, 10}, {15, 18}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort the array using -&gt; ex Arrays.sort(intervals, (arr1), (arr2) -&gt; Interger.compare(arr1[0], arr[1])) 
+Need to create a list of int[] because we don't know the size at runtime bc of merges.  Have a pointer to current_interval OUTSIDE of loop.  In loop, If you need to add an array to output, first set current_interval given interval array and add current_int to output. Merge:  current_int[1] = Math.max(currHigh, nextHigh) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given an array of Strings, return a list of arrays with where a given array is anagrams of eachother
+Input -&gt; strs = ["eat", "tea", "tan", "ate", "nat", "bat"]  
+Output -&gt; [["bat"], ["nat", "tan"], ["ate", "eat", "tea"] </t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -610,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -635,10 +635,10 @@
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>